<commit_message>
now it works widesmiley
</commit_message>
<xml_diff>
--- a/indikatoren_timeRandomized.xlsx
+++ b/indikatoren_timeRandomized.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaydi\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaydi\Desktop\Projekt_2023\Projekt2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24F660B6-5E97-4736-8EE7-6741A6FA82CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE64939F-0A0F-4D65-96D2-BFAD2C92553D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="2745" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1282,7 +1282,7 @@
   <dimension ref="A1:H286"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="T14" sqref="T14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1331,10 +1331,10 @@
         <v>294</v>
       </c>
       <c r="G2">
-        <v>5</v>
+        <v>4.7110987790000003</v>
       </c>
       <c r="H2">
-        <v>3</v>
+        <v>2.731553194</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1357,10 +1357,10 @@
         <v>294</v>
       </c>
       <c r="G3">
-        <v>4</v>
+        <v>4.0261884590000001</v>
       </c>
       <c r="H3">
-        <v>4</v>
+        <v>3.781229057</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1383,10 +1383,10 @@
         <v>294</v>
       </c>
       <c r="G4">
-        <v>5</v>
+        <v>4.8707415459999996</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>0.97658765400000003</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1409,10 +1409,10 @@
         <v>294</v>
       </c>
       <c r="G5">
-        <v>4</v>
+        <v>4.1754161129999998</v>
       </c>
       <c r="H5">
-        <v>2</v>
+        <v>1.8014413010000001</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1435,10 +1435,10 @@
         <v>294</v>
       </c>
       <c r="G6">
-        <v>3</v>
+        <v>3.0731554769999998</v>
       </c>
       <c r="H6">
-        <v>3</v>
+        <v>3.0993574279999998</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1461,10 +1461,10 @@
         <v>294</v>
       </c>
       <c r="G7">
-        <v>3</v>
+        <v>3.2971512170000001</v>
       </c>
       <c r="H7">
-        <v>3</v>
+        <v>3.2352170500000001</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1487,10 +1487,10 @@
         <v>295</v>
       </c>
       <c r="G8">
-        <v>5</v>
+        <v>4.8751290139999996</v>
       </c>
       <c r="H8">
-        <v>5</v>
+        <v>4.7894128010000001</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1513,10 +1513,10 @@
         <v>296</v>
       </c>
       <c r="G9">
-        <v>5</v>
+        <v>4.926891178</v>
       </c>
       <c r="H9">
-        <v>2</v>
+        <v>2.0976858040000002</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1539,10 +1539,10 @@
         <v>294</v>
       </c>
       <c r="G10">
-        <v>5</v>
+        <v>4.7465537119999999</v>
       </c>
       <c r="H10">
-        <v>3</v>
+        <v>2.74492344</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1565,10 +1565,10 @@
         <v>294</v>
       </c>
       <c r="G11">
-        <v>3</v>
+        <v>3.296890484</v>
       </c>
       <c r="H11">
-        <v>5</v>
+        <v>4.7480531560000001</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1591,10 +1591,10 @@
         <v>294</v>
       </c>
       <c r="G12">
-        <v>2</v>
+        <v>2.217191658</v>
       </c>
       <c r="H12">
-        <v>5</v>
+        <v>4.8160461379999999</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1617,10 +1617,10 @@
         <v>294</v>
       </c>
       <c r="G13">
-        <v>4</v>
+        <v>3.861419245</v>
       </c>
       <c r="H13">
-        <v>5</v>
+        <v>4.9170027699999999</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1643,10 +1643,10 @@
         <v>294</v>
       </c>
       <c r="G14">
-        <v>3</v>
+        <v>3.0923075770000001</v>
       </c>
       <c r="H14">
-        <v>3</v>
+        <v>3.0378559740000002</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1669,10 +1669,10 @@
         <v>295</v>
       </c>
       <c r="G15">
-        <v>4</v>
+        <v>3.8360509399999998</v>
       </c>
       <c r="H15">
-        <v>4</v>
+        <v>3.995942849</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1695,10 +1695,10 @@
         <v>295</v>
       </c>
       <c r="G16">
-        <v>4</v>
+        <v>3.708752488</v>
       </c>
       <c r="H16">
-        <v>5</v>
+        <v>4.7895726920000001</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1721,10 +1721,10 @@
         <v>294</v>
       </c>
       <c r="G17">
-        <v>2</v>
+        <v>1.7984392380000001</v>
       </c>
       <c r="H17">
-        <v>4</v>
+        <v>4.2239162600000002</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1747,10 +1747,10 @@
         <v>295</v>
       </c>
       <c r="G18">
-        <v>3</v>
+        <v>3.0283611270000002</v>
       </c>
       <c r="H18">
-        <v>3</v>
+        <v>2.9918217629999999</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1773,10 +1773,10 @@
         <v>295</v>
       </c>
       <c r="G19">
-        <v>4</v>
+        <v>3.7144704220000002</v>
       </c>
       <c r="H19">
-        <v>2</v>
+        <v>1.8541666750000001</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1799,10 +1799,10 @@
         <v>294</v>
       </c>
       <c r="G20">
-        <v>4</v>
+        <v>4.1267996299999998</v>
       </c>
       <c r="H20">
-        <v>2</v>
+        <v>1.9055699269999999</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1825,10 +1825,10 @@
         <v>295</v>
       </c>
       <c r="G21">
-        <v>3</v>
+        <v>3.1864049040000002</v>
       </c>
       <c r="H21">
-        <v>5</v>
+        <v>4.7657701149999996</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1851,10 +1851,10 @@
         <v>294</v>
       </c>
       <c r="G22">
-        <v>1</v>
+        <v>1.0222028270000001</v>
       </c>
       <c r="H22">
-        <v>3</v>
+        <v>3.0485487419999999</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1877,10 +1877,10 @@
         <v>296</v>
       </c>
       <c r="G23">
-        <v>3</v>
+        <v>3.1023838989999999</v>
       </c>
       <c r="H23">
-        <v>2</v>
+        <v>1.963232614</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1903,10 +1903,10 @@
         <v>295</v>
       </c>
       <c r="G24">
-        <v>4</v>
+        <v>3.9421003780000001</v>
       </c>
       <c r="H24">
-        <v>2</v>
+        <v>1.947355301</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1929,10 +1929,10 @@
         <v>295</v>
       </c>
       <c r="G25">
-        <v>3</v>
+        <v>2.824859038</v>
       </c>
       <c r="H25">
-        <v>4</v>
+        <v>3.9600295430000001</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1955,10 +1955,10 @@
         <v>296</v>
       </c>
       <c r="G26">
-        <v>4</v>
+        <v>4.2335471150000004</v>
       </c>
       <c r="H26">
-        <v>4</v>
+        <v>4.0686693109999998</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1981,10 +1981,10 @@
         <v>296</v>
       </c>
       <c r="G27">
-        <v>3</v>
+        <v>2.838297533</v>
       </c>
       <c r="H27">
-        <v>3</v>
+        <v>3.2897204360000001</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -2007,10 +2007,10 @@
         <v>296</v>
       </c>
       <c r="G28">
-        <v>5</v>
+        <v>4.867713706</v>
       </c>
       <c r="H28">
-        <v>2</v>
+        <v>2.0528759779999999</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -2033,10 +2033,10 @@
         <v>294</v>
       </c>
       <c r="G29">
-        <v>3</v>
+        <v>3.1977255699999998</v>
       </c>
       <c r="H29">
-        <v>4</v>
+        <v>4.2086848520000002</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -2059,10 +2059,10 @@
         <v>294</v>
       </c>
       <c r="G30">
-        <v>3</v>
+        <v>2.8128671839999999</v>
       </c>
       <c r="H30">
-        <v>4</v>
+        <v>3.9959863580000001</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -2085,10 +2085,10 @@
         <v>295</v>
       </c>
       <c r="G31">
-        <v>3</v>
+        <v>2.9695793909999999</v>
       </c>
       <c r="H31">
-        <v>5</v>
+        <v>4.9257828420000003</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -2111,10 +2111,10 @@
         <v>294</v>
       </c>
       <c r="G32">
-        <v>5</v>
+        <v>4.7946234260000002</v>
       </c>
       <c r="H32">
-        <v>4</v>
+        <v>3.8000621909999999</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -2137,10 +2137,10 @@
         <v>296</v>
       </c>
       <c r="G33">
-        <v>3</v>
+        <v>3.1115999620000001</v>
       </c>
       <c r="H33">
-        <v>2</v>
+        <v>1.9263126079999999</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -2163,10 +2163,10 @@
         <v>294</v>
       </c>
       <c r="G34">
-        <v>2</v>
+        <v>1.954825743</v>
       </c>
       <c r="H34">
-        <v>2</v>
+        <v>1.777959587</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -2189,10 +2189,10 @@
         <v>296</v>
       </c>
       <c r="G35">
-        <v>3</v>
+        <v>3.1398164469999998</v>
       </c>
       <c r="H35">
-        <v>2</v>
+        <v>1.7359319179999999</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -2215,10 +2215,10 @@
         <v>295</v>
       </c>
       <c r="G36">
-        <v>4</v>
+        <v>4.0615497429999996</v>
       </c>
       <c r="H36">
-        <v>5</v>
+        <v>4.9859377990000002</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -2244,7 +2244,7 @@
         <v>5</v>
       </c>
       <c r="H37">
-        <v>2</v>
+        <v>1.887204812</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -2267,10 +2267,10 @@
         <v>296</v>
       </c>
       <c r="G38">
-        <v>2</v>
+        <v>1.8219789609999999</v>
       </c>
       <c r="H38">
-        <v>2</v>
+        <v>1.860477068</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -2293,10 +2293,10 @@
         <v>296</v>
       </c>
       <c r="G39">
-        <v>3</v>
+        <v>3.1150970230000001</v>
       </c>
       <c r="H39">
-        <v>2</v>
+        <v>1.9628278880000001</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -2319,10 +2319,10 @@
         <v>294</v>
       </c>
       <c r="G40">
-        <v>3</v>
+        <v>3.1682322100000002</v>
       </c>
       <c r="H40">
-        <v>5</v>
+        <v>4.8051274470000003</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -2345,10 +2345,10 @@
         <v>296</v>
       </c>
       <c r="G41">
-        <v>5</v>
+        <v>4.8287266259999999</v>
       </c>
       <c r="H41">
-        <v>3</v>
+        <v>2.8602723700000001</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -2371,10 +2371,10 @@
         <v>296</v>
       </c>
       <c r="G42">
-        <v>2</v>
+        <v>1.7313059850000001</v>
       </c>
       <c r="H42">
-        <v>1</v>
+        <v>0.97635456200000004</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -2397,10 +2397,10 @@
         <v>296</v>
       </c>
       <c r="G43">
-        <v>4</v>
+        <v>4.0395843779999998</v>
       </c>
       <c r="H43">
-        <v>3</v>
+        <v>2.7564577680000002</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -2423,10 +2423,10 @@
         <v>296</v>
       </c>
       <c r="G44">
-        <v>4</v>
+        <v>3.8395990539999998</v>
       </c>
       <c r="H44">
-        <v>4</v>
+        <v>3.8520898840000002</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -2449,10 +2449,10 @@
         <v>296</v>
       </c>
       <c r="G45">
-        <v>3</v>
+        <v>2.7458383450000001</v>
       </c>
       <c r="H45">
-        <v>2</v>
+        <v>1.7755176800000001</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -2475,10 +2475,10 @@
         <v>295</v>
       </c>
       <c r="G46">
-        <v>3</v>
+        <v>2.9037028550000001</v>
       </c>
       <c r="H46">
-        <v>3</v>
+        <v>3.183098083</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -2501,10 +2501,10 @@
         <v>296</v>
       </c>
       <c r="G47">
-        <v>2</v>
+        <v>1.966798539</v>
       </c>
       <c r="H47">
-        <v>2</v>
+        <v>2.25957922</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -2527,10 +2527,10 @@
         <v>296</v>
       </c>
       <c r="G48">
-        <v>2</v>
+        <v>1.7555968980000001</v>
       </c>
       <c r="H48">
-        <v>3</v>
+        <v>3.1731167980000001</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -2553,10 +2553,10 @@
         <v>296</v>
       </c>
       <c r="G49">
-        <v>5</v>
+        <v>4.9235751929999996</v>
       </c>
       <c r="H49">
-        <v>2</v>
+        <v>2.0247157740000001</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -2579,10 +2579,10 @@
         <v>296</v>
       </c>
       <c r="G50">
-        <v>5</v>
+        <v>4.8488654369999997</v>
       </c>
       <c r="H50">
-        <v>4</v>
+        <v>3.9772195809999999</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -2605,10 +2605,10 @@
         <v>295</v>
       </c>
       <c r="G51">
-        <v>5</v>
+        <v>4.7758846110000004</v>
       </c>
       <c r="H51">
-        <v>3</v>
+        <v>3.052564667</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -2631,10 +2631,10 @@
         <v>296</v>
       </c>
       <c r="G52">
-        <v>5</v>
+        <v>4.9980562260000001</v>
       </c>
       <c r="H52">
-        <v>5</v>
+        <v>4.7691831249999996</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -2657,10 +2657,10 @@
         <v>295</v>
       </c>
       <c r="G53">
-        <v>4</v>
+        <v>4.2404434770000003</v>
       </c>
       <c r="H53">
-        <v>3</v>
+        <v>2.768924417</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -2683,10 +2683,10 @@
         <v>295</v>
       </c>
       <c r="G54">
-        <v>5</v>
+        <v>4.9051435379999999</v>
       </c>
       <c r="H54">
-        <v>3</v>
+        <v>2.9617325700000001</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -2709,10 +2709,10 @@
         <v>295</v>
       </c>
       <c r="G55">
-        <v>5</v>
+        <v>4.9062075639999998</v>
       </c>
       <c r="H55">
-        <v>4</v>
+        <v>3.7248379749999998</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -2735,10 +2735,10 @@
         <v>295</v>
       </c>
       <c r="G56">
-        <v>5</v>
+        <v>4.8781357359999999</v>
       </c>
       <c r="H56">
-        <v>3</v>
+        <v>2.9721823359999999</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -2761,10 +2761,10 @@
         <v>296</v>
       </c>
       <c r="G57">
-        <v>5</v>
+        <v>4.902513645</v>
       </c>
       <c r="H57">
-        <v>3</v>
+        <v>2.7422927459999999</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -2787,10 +2787,10 @@
         <v>296</v>
       </c>
       <c r="G58">
-        <v>5</v>
+        <v>4.8712384389999999</v>
       </c>
       <c r="H58">
-        <v>3</v>
+        <v>3.009434063</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
@@ -2813,10 +2813,10 @@
         <v>296</v>
       </c>
       <c r="G59">
-        <v>5</v>
+        <v>4.960962952</v>
       </c>
       <c r="H59">
-        <v>4</v>
+        <v>4.0232216850000002</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -2839,10 +2839,10 @@
         <v>294</v>
       </c>
       <c r="G60">
-        <v>3</v>
+        <v>2.7833836019999998</v>
       </c>
       <c r="H60">
-        <v>5</v>
+        <v>4.8583031090000004</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
@@ -2865,10 +2865,10 @@
         <v>295</v>
       </c>
       <c r="G61">
-        <v>5</v>
+        <v>4.9494485419999998</v>
       </c>
       <c r="H61">
-        <v>3</v>
+        <v>2.8455595690000002</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
@@ -2891,10 +2891,10 @@
         <v>295</v>
       </c>
       <c r="G62">
-        <v>5</v>
+        <v>4.7010621849999996</v>
       </c>
       <c r="H62">
-        <v>4</v>
+        <v>3.9163485570000001</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
@@ -2917,10 +2917,10 @@
         <v>295</v>
       </c>
       <c r="G63">
-        <v>3</v>
+        <v>3.1856900640000001</v>
       </c>
       <c r="H63">
-        <v>2</v>
+        <v>2.0272398960000002</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
@@ -2943,10 +2943,10 @@
         <v>295</v>
       </c>
       <c r="G64">
-        <v>5</v>
+        <v>4.9541594839999998</v>
       </c>
       <c r="H64">
-        <v>1</v>
+        <v>1.005995244</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
@@ -2969,10 +2969,10 @@
         <v>295</v>
       </c>
       <c r="G65">
-        <v>3</v>
+        <v>3.0250653320000001</v>
       </c>
       <c r="H65">
-        <v>4</v>
+        <v>3.7562950449999999</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -2995,10 +2995,10 @@
         <v>294</v>
       </c>
       <c r="G66">
-        <v>3</v>
+        <v>2.7863314950000002</v>
       </c>
       <c r="H66">
-        <v>5</v>
+        <v>4.7235045370000002</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
@@ -3021,10 +3021,10 @@
         <v>296</v>
       </c>
       <c r="G67">
-        <v>4</v>
+        <v>3.9144170470000001</v>
       </c>
       <c r="H67">
-        <v>3</v>
+        <v>3.0703875900000002</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
@@ -3047,10 +3047,10 @@
         <v>295</v>
       </c>
       <c r="G68">
-        <v>5</v>
+        <v>4.8270044529999998</v>
       </c>
       <c r="H68">
-        <v>1</v>
+        <v>0.72685386399999996</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
@@ -3073,10 +3073,10 @@
         <v>296</v>
       </c>
       <c r="G69">
-        <v>5</v>
+        <v>4.8666583619999999</v>
       </c>
       <c r="H69">
-        <v>4</v>
+        <v>4.2542429310000003</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
@@ -3099,10 +3099,10 @@
         <v>295</v>
       </c>
       <c r="G70">
-        <v>5</v>
+        <v>4.9369150169999996</v>
       </c>
       <c r="H70">
-        <v>1</v>
+        <v>0.93224044900000003</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
@@ -3125,10 +3125,10 @@
         <v>296</v>
       </c>
       <c r="G71">
-        <v>5</v>
+        <v>4.9361086429999999</v>
       </c>
       <c r="H71">
-        <v>3</v>
+        <v>2.7960070770000001</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
@@ -3151,10 +3151,10 @@
         <v>296</v>
       </c>
       <c r="G72">
-        <v>5</v>
+        <v>4.9598324700000003</v>
       </c>
       <c r="H72">
-        <v>3</v>
+        <v>3.1048366810000001</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
@@ -3177,10 +3177,10 @@
         <v>295</v>
       </c>
       <c r="G73">
-        <v>3</v>
+        <v>2.8501881849999999</v>
       </c>
       <c r="H73">
-        <v>3</v>
+        <v>3.2610329720000002</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
@@ -3203,10 +3203,10 @@
         <v>294</v>
       </c>
       <c r="G74">
-        <v>4</v>
+        <v>3.846273976</v>
       </c>
       <c r="H74">
-        <v>4</v>
+        <v>3.8516490659999998</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -3229,10 +3229,10 @@
         <v>296</v>
       </c>
       <c r="G75">
-        <v>4</v>
+        <v>4.029020364</v>
       </c>
       <c r="H75">
-        <v>4</v>
+        <v>4.1567294390000002</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -3255,10 +3255,10 @@
         <v>296</v>
       </c>
       <c r="G76">
-        <v>2</v>
+        <v>1.8768809019999999</v>
       </c>
       <c r="H76">
-        <v>2</v>
+        <v>1.8805539819999999</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -3281,10 +3281,10 @@
         <v>294</v>
       </c>
       <c r="G77">
-        <v>4</v>
+        <v>4.097001423</v>
       </c>
       <c r="H77">
-        <v>4</v>
+        <v>4.0048654060000004</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
@@ -3307,10 +3307,10 @@
         <v>294</v>
       </c>
       <c r="G78">
-        <v>3</v>
+        <v>2.9612338199999999</v>
       </c>
       <c r="H78">
-        <v>5</v>
+        <v>4.8209073719999997</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
@@ -3333,10 +3333,10 @@
         <v>294</v>
       </c>
       <c r="G79">
-        <v>2</v>
+        <v>1.7742044340000001</v>
       </c>
       <c r="H79">
-        <v>1</v>
+        <v>0.83103716299999997</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
@@ -3359,10 +3359,10 @@
         <v>295</v>
       </c>
       <c r="G80">
-        <v>3</v>
+        <v>2.8332873279999999</v>
       </c>
       <c r="H80">
-        <v>3</v>
+        <v>3.080068282</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
@@ -3385,10 +3385,10 @@
         <v>294</v>
       </c>
       <c r="G81">
-        <v>2</v>
+        <v>2.2169023650000002</v>
       </c>
       <c r="H81">
-        <v>4</v>
+        <v>4.1602957189999996</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
@@ -3411,10 +3411,10 @@
         <v>296</v>
       </c>
       <c r="G82">
-        <v>4</v>
+        <v>3.8946610160000001</v>
       </c>
       <c r="H82">
-        <v>2</v>
+        <v>2.1517248809999998</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
@@ -3437,10 +3437,10 @@
         <v>294</v>
       </c>
       <c r="G83">
-        <v>2</v>
+        <v>2.089773879</v>
       </c>
       <c r="H83">
-        <v>4</v>
+        <v>3.8878618870000001</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
@@ -3463,10 +3463,10 @@
         <v>295</v>
       </c>
       <c r="G84">
-        <v>3</v>
+        <v>3.1352479130000002</v>
       </c>
       <c r="H84">
-        <v>4</v>
+        <v>3.8252526640000002</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
@@ -3489,10 +3489,10 @@
         <v>295</v>
       </c>
       <c r="G85">
-        <v>4</v>
+        <v>4.1813085210000001</v>
       </c>
       <c r="H85">
-        <v>2</v>
+        <v>2.0898883719999999</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
@@ -3515,10 +3515,10 @@
         <v>294</v>
       </c>
       <c r="G86">
-        <v>3</v>
+        <v>3.0947133500000001</v>
       </c>
       <c r="H86">
-        <v>4</v>
+        <v>4.0927428069999996</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
@@ -3541,10 +3541,10 @@
         <v>295</v>
       </c>
       <c r="G87">
-        <v>3</v>
+        <v>2.750414353</v>
       </c>
       <c r="H87">
-        <v>2</v>
+        <v>2.2285028680000001</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
@@ -3567,10 +3567,10 @@
         <v>294</v>
       </c>
       <c r="G88">
-        <v>1</v>
+        <v>0.86266358099999996</v>
       </c>
       <c r="H88">
-        <v>4</v>
+        <v>3.7548327800000001</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
@@ -3593,10 +3593,10 @@
         <v>295</v>
       </c>
       <c r="G89">
-        <v>3</v>
+        <v>3.1188416010000002</v>
       </c>
       <c r="H89">
-        <v>4</v>
+        <v>3.879416827</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
@@ -3619,10 +3619,10 @@
         <v>296</v>
       </c>
       <c r="G90">
-        <v>2</v>
+        <v>2.296065188</v>
       </c>
       <c r="H90">
-        <v>1</v>
+        <v>0.91821012800000001</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
@@ -3645,10 +3645,10 @@
         <v>296</v>
       </c>
       <c r="G91">
-        <v>3</v>
+        <v>3.099997181</v>
       </c>
       <c r="H91">
-        <v>1</v>
+        <v>0.70342118399999998</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
@@ -3671,10 +3671,10 @@
         <v>295</v>
       </c>
       <c r="G92">
-        <v>5</v>
+        <v>4.8440020190000004</v>
       </c>
       <c r="H92">
-        <v>4</v>
+        <v>4.1857544329999996</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
@@ -3697,10 +3697,10 @@
         <v>295</v>
       </c>
       <c r="G93">
-        <v>4</v>
+        <v>3.793889466</v>
       </c>
       <c r="H93">
-        <v>3</v>
+        <v>2.96573281</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
@@ -3723,10 +3723,10 @@
         <v>295</v>
       </c>
       <c r="G94">
-        <v>5</v>
+        <v>4.8287238500000003</v>
       </c>
       <c r="H94">
-        <v>5</v>
+        <v>4.7340702690000001</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
@@ -3749,10 +3749,10 @@
         <v>296</v>
       </c>
       <c r="G95">
-        <v>4</v>
+        <v>4.2622059070000002</v>
       </c>
       <c r="H95">
-        <v>4</v>
+        <v>4.1460737989999998</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
@@ -3775,10 +3775,10 @@
         <v>296</v>
       </c>
       <c r="G96">
-        <v>4</v>
+        <v>3.8646014320000002</v>
       </c>
       <c r="H96">
-        <v>5</v>
+        <v>4.8246590060000001</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
@@ -3801,10 +3801,10 @@
         <v>296</v>
       </c>
       <c r="G97">
-        <v>4</v>
+        <v>4.0568917979999997</v>
       </c>
       <c r="H97">
-        <v>4</v>
+        <v>3.9764515989999998</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
@@ -3827,10 +3827,10 @@
         <v>295</v>
       </c>
       <c r="G98">
-        <v>4</v>
+        <v>3.9792471040000001</v>
       </c>
       <c r="H98">
-        <v>1</v>
+        <v>1.2816802920000001</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
@@ -3853,10 +3853,10 @@
         <v>295</v>
       </c>
       <c r="G99">
-        <v>4</v>
+        <v>4.1107928080000002</v>
       </c>
       <c r="H99">
-        <v>3</v>
+        <v>2.7998490039999999</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
@@ -3879,10 +3879,10 @@
         <v>295</v>
       </c>
       <c r="G100">
-        <v>4</v>
+        <v>3.7184720910000002</v>
       </c>
       <c r="H100">
-        <v>1</v>
+        <v>0.96071589499999999</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
@@ -3905,10 +3905,10 @@
         <v>295</v>
       </c>
       <c r="G101">
-        <v>4</v>
+        <v>3.8041610509999999</v>
       </c>
       <c r="H101">
-        <v>4</v>
+        <v>3.89069624</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
@@ -3931,10 +3931,10 @@
         <v>295</v>
       </c>
       <c r="G102">
-        <v>4</v>
+        <v>4.1274962149999999</v>
       </c>
       <c r="H102">
-        <v>1</v>
+        <v>1.122205366</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
@@ -3957,10 +3957,10 @@
         <v>294</v>
       </c>
       <c r="G103">
-        <v>2</v>
+        <v>1.76140392</v>
       </c>
       <c r="H103">
-        <v>2</v>
+        <v>2.1224567790000002</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
@@ -3983,10 +3983,10 @@
         <v>294</v>
       </c>
       <c r="G104">
-        <v>1</v>
+        <v>0.95090103599999998</v>
       </c>
       <c r="H104">
-        <v>1</v>
+        <v>1.1871340079999999</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
@@ -4009,10 +4009,10 @@
         <v>294</v>
       </c>
       <c r="G105">
-        <v>2</v>
+        <v>2.2373017320000002</v>
       </c>
       <c r="H105">
-        <v>1</v>
+        <v>1.0699524840000001</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
@@ -4035,10 +4035,10 @@
         <v>295</v>
       </c>
       <c r="G106">
-        <v>2</v>
+        <v>1.7768511849999999</v>
       </c>
       <c r="H106">
-        <v>1</v>
+        <v>0.82757097300000004</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
@@ -4061,10 +4061,10 @@
         <v>296</v>
       </c>
       <c r="G107">
-        <v>3</v>
+        <v>2.9253755400000001</v>
       </c>
       <c r="H107">
-        <v>2</v>
+        <v>1.882633118</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
@@ -4087,10 +4087,10 @@
         <v>296</v>
       </c>
       <c r="G108">
-        <v>5</v>
+        <v>4.9039021140000001</v>
       </c>
       <c r="H108">
-        <v>4</v>
+        <v>4.031594492</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
@@ -4113,10 +4113,10 @@
         <v>296</v>
       </c>
       <c r="G109">
-        <v>2</v>
+        <v>1.8441651100000001</v>
       </c>
       <c r="H109">
-        <v>2</v>
+        <v>2.1659244590000002</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
@@ -4139,10 +4139,10 @@
         <v>295</v>
       </c>
       <c r="G110">
-        <v>2</v>
+        <v>1.7412069240000001</v>
       </c>
       <c r="H110">
-        <v>5</v>
+        <v>4.727370359</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
@@ -4165,10 +4165,10 @@
         <v>296</v>
       </c>
       <c r="G111">
-        <v>4</v>
+        <v>4.1902927229999998</v>
       </c>
       <c r="H111">
-        <v>3</v>
+        <v>2.8737322870000002</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
@@ -4191,10 +4191,10 @@
         <v>294</v>
       </c>
       <c r="G112">
-        <v>2</v>
+        <v>1.983998312</v>
       </c>
       <c r="H112">
-        <v>4</v>
+        <v>3.9171714519999998</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
@@ -4217,10 +4217,10 @@
         <v>294</v>
       </c>
       <c r="G113">
-        <v>1</v>
+        <v>0.93221625100000005</v>
       </c>
       <c r="H113">
-        <v>1</v>
+        <v>1.2938606989999999</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
@@ -4243,10 +4243,10 @@
         <v>295</v>
       </c>
       <c r="G114">
-        <v>5</v>
+        <v>4.7084501479999998</v>
       </c>
       <c r="H114">
-        <v>5</v>
+        <v>4.8442373070000002</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
@@ -4269,10 +4269,10 @@
         <v>294</v>
       </c>
       <c r="G115">
-        <v>3</v>
+        <v>2.9003393609999999</v>
       </c>
       <c r="H115">
-        <v>2</v>
+        <v>2.1125700329999999</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
@@ -4295,10 +4295,10 @@
         <v>296</v>
       </c>
       <c r="G116">
-        <v>5</v>
+        <v>4.8862876330000002</v>
       </c>
       <c r="H116">
-        <v>2</v>
+        <v>1.8421507859999999</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
@@ -4321,10 +4321,10 @@
         <v>296</v>
       </c>
       <c r="G117">
-        <v>4</v>
+        <v>3.830684148</v>
       </c>
       <c r="H117">
-        <v>4</v>
+        <v>3.7936699900000002</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
@@ -4347,10 +4347,10 @@
         <v>296</v>
       </c>
       <c r="G118">
-        <v>2</v>
+        <v>1.902617432</v>
       </c>
       <c r="H118">
-        <v>2</v>
+        <v>2.2810320989999999</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
@@ -4373,10 +4373,10 @@
         <v>295</v>
       </c>
       <c r="G119">
-        <v>3</v>
+        <v>2.8668165480000001</v>
       </c>
       <c r="H119">
-        <v>1</v>
+        <v>0.93095319799999998</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
@@ -4399,10 +4399,10 @@
         <v>296</v>
       </c>
       <c r="G120">
-        <v>3</v>
+        <v>2.902373898</v>
       </c>
       <c r="H120">
-        <v>2</v>
+        <v>1.7614400779999999</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
@@ -4425,10 +4425,10 @@
         <v>294</v>
       </c>
       <c r="G121">
-        <v>2</v>
+        <v>1.812053505</v>
       </c>
       <c r="H121">
-        <v>2</v>
+        <v>1.7753701710000001</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
@@ -4451,10 +4451,10 @@
         <v>294</v>
       </c>
       <c r="G122">
-        <v>3</v>
+        <v>3.0544659510000001</v>
       </c>
       <c r="H122">
-        <v>1</v>
+        <v>1.1061160569999999</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
@@ -4477,7 +4477,7 @@
         <v>294</v>
       </c>
       <c r="G123">
-        <v>2</v>
+        <v>2.0818925739999998</v>
       </c>
       <c r="H123">
         <v>5</v>
@@ -4503,10 +4503,10 @@
         <v>296</v>
       </c>
       <c r="G124">
-        <v>4</v>
+        <v>4.1997942119999996</v>
       </c>
       <c r="H124">
-        <v>1</v>
+        <v>0.741441448</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
@@ -4529,10 +4529,10 @@
         <v>294</v>
       </c>
       <c r="G125">
-        <v>3</v>
+        <v>2.953408638</v>
       </c>
       <c r="H125">
-        <v>2</v>
+        <v>1.7479512859999999</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
@@ -4555,10 +4555,10 @@
         <v>295</v>
       </c>
       <c r="G126">
-        <v>3</v>
+        <v>3.1522187920000002</v>
       </c>
       <c r="H126">
-        <v>2</v>
+        <v>1.8080116369999999</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
@@ -4581,10 +4581,10 @@
         <v>295</v>
       </c>
       <c r="G127">
-        <v>3</v>
+        <v>3.078038662</v>
       </c>
       <c r="H127">
-        <v>3</v>
+        <v>3.2571671809999998</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
@@ -4607,10 +4607,10 @@
         <v>295</v>
       </c>
       <c r="G128">
-        <v>3</v>
+        <v>3.1799133510000002</v>
       </c>
       <c r="H128">
-        <v>5</v>
+        <v>4.956517614</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
@@ -4633,10 +4633,10 @@
         <v>294</v>
       </c>
       <c r="G129">
-        <v>2</v>
+        <v>2.0886166589999999</v>
       </c>
       <c r="H129">
-        <v>2</v>
+        <v>2.176758247</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
@@ -4659,10 +4659,10 @@
         <v>295</v>
       </c>
       <c r="G130">
-        <v>3</v>
+        <v>2.8787424850000001</v>
       </c>
       <c r="H130">
-        <v>2</v>
+        <v>1.746664754</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
@@ -4685,10 +4685,10 @@
         <v>295</v>
       </c>
       <c r="G131">
-        <v>3</v>
+        <v>3.150123115</v>
       </c>
       <c r="H131">
-        <v>2</v>
+        <v>1.955774444</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
@@ -4711,10 +4711,10 @@
         <v>294</v>
       </c>
       <c r="G132">
-        <v>1</v>
+        <v>1.0557466630000001</v>
       </c>
       <c r="H132">
-        <v>1</v>
+        <v>1.225631701</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
@@ -4737,10 +4737,10 @@
         <v>294</v>
       </c>
       <c r="G133">
-        <v>1</v>
+        <v>1.17525843</v>
       </c>
       <c r="H133">
-        <v>1</v>
+        <v>0.71703860799999997</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
@@ -4763,10 +4763,10 @@
         <v>296</v>
       </c>
       <c r="G134">
-        <v>3</v>
+        <v>2.7267593450000001</v>
       </c>
       <c r="H134">
-        <v>4</v>
+        <v>4.1661263220000002</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
@@ -4789,10 +4789,10 @@
         <v>294</v>
       </c>
       <c r="G135">
-        <v>2</v>
+        <v>2.0113545309999998</v>
       </c>
       <c r="H135">
-        <v>1</v>
+        <v>0.72885215999999997</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
@@ -4815,10 +4815,10 @@
         <v>294</v>
       </c>
       <c r="G136">
-        <v>1</v>
+        <v>1.034805091</v>
       </c>
       <c r="H136">
-        <v>1</v>
+        <v>0.70787900800000003</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
@@ -4841,10 +4841,10 @@
         <v>295</v>
       </c>
       <c r="G137">
-        <v>1</v>
+        <v>0.98252775199999998</v>
       </c>
       <c r="H137">
-        <v>1</v>
+        <v>1.139325221</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
@@ -4867,10 +4867,10 @@
         <v>296</v>
       </c>
       <c r="G138">
-        <v>4</v>
+        <v>4.0603755359999996</v>
       </c>
       <c r="H138">
-        <v>3</v>
+        <v>2.7438314899999998</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
@@ -4893,10 +4893,10 @@
         <v>296</v>
       </c>
       <c r="G139">
-        <v>3</v>
+        <v>2.8801356029999998</v>
       </c>
       <c r="H139">
-        <v>1</v>
+        <v>0.71624598500000003</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
@@ -4919,10 +4919,10 @@
         <v>294</v>
       </c>
       <c r="G140">
-        <v>1</v>
+        <v>1.267542189</v>
       </c>
       <c r="H140">
-        <v>3</v>
+        <v>3.0797699180000002</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.25">
@@ -4945,10 +4945,10 @@
         <v>295</v>
       </c>
       <c r="G141">
-        <v>1</v>
+        <v>0.712188355</v>
       </c>
       <c r="H141">
-        <v>3</v>
+        <v>2.7616103729999999</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
@@ -4971,10 +4971,10 @@
         <v>296</v>
       </c>
       <c r="G142">
-        <v>5</v>
+        <v>4.7138106679999998</v>
       </c>
       <c r="H142">
-        <v>5</v>
+        <v>4.9764271869999996</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
@@ -4997,10 +4997,10 @@
         <v>296</v>
       </c>
       <c r="G143">
-        <v>4</v>
+        <v>4.0106138979999999</v>
       </c>
       <c r="H143">
-        <v>2</v>
+        <v>1.902630705</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
@@ -5023,10 +5023,10 @@
         <v>295</v>
       </c>
       <c r="G144">
-        <v>3</v>
+        <v>3.2832045519999999</v>
       </c>
       <c r="H144">
-        <v>1</v>
+        <v>0.85958018000000003</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
@@ -5049,10 +5049,10 @@
         <v>296</v>
       </c>
       <c r="G145">
-        <v>5</v>
+        <v>4.9482908820000002</v>
       </c>
       <c r="H145">
-        <v>3</v>
+        <v>3.0370176780000002</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.25">
@@ -5075,10 +5075,10 @@
         <v>295</v>
       </c>
       <c r="G146">
-        <v>4</v>
+        <v>4.0948962440000001</v>
       </c>
       <c r="H146">
-        <v>1</v>
+        <v>0.91440174100000005</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.25">
@@ -5101,10 +5101,10 @@
         <v>295</v>
       </c>
       <c r="G147">
-        <v>4</v>
+        <v>3.7037378159999998</v>
       </c>
       <c r="H147">
-        <v>4</v>
+        <v>3.824675628</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.25">
@@ -5127,10 +5127,10 @@
         <v>295</v>
       </c>
       <c r="G148">
-        <v>5</v>
+        <v>4.8847493850000001</v>
       </c>
       <c r="H148">
-        <v>3</v>
+        <v>3.2081946779999999</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.25">
@@ -5153,10 +5153,10 @@
         <v>296</v>
       </c>
       <c r="G149">
-        <v>5</v>
+        <v>4.8084385709999999</v>
       </c>
       <c r="H149">
-        <v>4</v>
+        <v>3.984354519</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
@@ -5179,10 +5179,10 @@
         <v>294</v>
       </c>
       <c r="G150">
-        <v>3</v>
+        <v>3.0715805129999998</v>
       </c>
       <c r="H150">
-        <v>2</v>
+        <v>2.0277956779999999</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.25">
@@ -5205,10 +5205,10 @@
         <v>296</v>
       </c>
       <c r="G151">
-        <v>5</v>
+        <v>4.8494201319999997</v>
       </c>
       <c r="H151">
-        <v>3</v>
+        <v>2.9741449640000002</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.25">
@@ -5231,10 +5231,10 @@
         <v>296</v>
       </c>
       <c r="G152">
-        <v>4</v>
+        <v>3.8152766630000001</v>
       </c>
       <c r="H152">
-        <v>2</v>
+        <v>1.958236154</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.25">
@@ -5257,10 +5257,10 @@
         <v>296</v>
       </c>
       <c r="G153">
-        <v>4</v>
+        <v>4.2290200200000001</v>
       </c>
       <c r="H153">
-        <v>5</v>
+        <v>4.7256003020000001</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
@@ -5283,10 +5283,10 @@
         <v>296</v>
       </c>
       <c r="G154">
-        <v>5</v>
+        <v>4.8028648069999997</v>
       </c>
       <c r="H154">
-        <v>3</v>
+        <v>3.0877918819999999</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.25">
@@ -5309,10 +5309,10 @@
         <v>295</v>
       </c>
       <c r="G155">
-        <v>2</v>
+        <v>1.965561503</v>
       </c>
       <c r="H155">
-        <v>1</v>
+        <v>1.2138726040000001</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
@@ -5338,7 +5338,7 @@
         <v>5</v>
       </c>
       <c r="H156">
-        <v>3</v>
+        <v>3.1967800639999999</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.25">
@@ -5361,10 +5361,10 @@
         <v>294</v>
       </c>
       <c r="G157">
-        <v>1</v>
+        <v>0.98742903100000001</v>
       </c>
       <c r="H157">
-        <v>1</v>
+        <v>0.76525508799999997</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.25">
@@ -5387,10 +5387,10 @@
         <v>296</v>
       </c>
       <c r="G158">
-        <v>5</v>
+        <v>4.998943283</v>
       </c>
       <c r="H158">
-        <v>3</v>
+        <v>3.134245376</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
@@ -5413,10 +5413,10 @@
         <v>296</v>
       </c>
       <c r="G159">
-        <v>4</v>
+        <v>3.8309269979999998</v>
       </c>
       <c r="H159">
-        <v>2</v>
+        <v>1.7235508369999999</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.25">
@@ -5439,10 +5439,10 @@
         <v>294</v>
       </c>
       <c r="G160">
-        <v>2</v>
+        <v>1.9592216769999999</v>
       </c>
       <c r="H160">
-        <v>3</v>
+        <v>3.1857559379999998</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.25">
@@ -5465,10 +5465,10 @@
         <v>296</v>
       </c>
       <c r="G161">
-        <v>5</v>
+        <v>4.9203854250000001</v>
       </c>
       <c r="H161">
-        <v>3</v>
+        <v>2.7709583750000002</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.25">
@@ -5491,10 +5491,10 @@
         <v>296</v>
       </c>
       <c r="G162">
-        <v>4</v>
+        <v>3.9034986859999998</v>
       </c>
       <c r="H162">
-        <v>4</v>
+        <v>4.112246142</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.25">
@@ -5517,10 +5517,10 @@
         <v>295</v>
       </c>
       <c r="G163">
-        <v>5</v>
+        <v>4.9717762780000001</v>
       </c>
       <c r="H163">
-        <v>4</v>
+        <v>3.9720385230000002</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.25">
@@ -5543,10 +5543,10 @@
         <v>296</v>
       </c>
       <c r="G164">
-        <v>3</v>
+        <v>3.2501997810000001</v>
       </c>
       <c r="H164">
-        <v>2</v>
+        <v>1.759223559</v>
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.25">
@@ -5569,10 +5569,10 @@
         <v>296</v>
       </c>
       <c r="G165">
-        <v>5</v>
+        <v>4.9732715079999998</v>
       </c>
       <c r="H165">
-        <v>5</v>
+        <v>4.9114686980000002</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.25">
@@ -5595,10 +5595,10 @@
         <v>296</v>
       </c>
       <c r="G166">
-        <v>4</v>
+        <v>3.946707172</v>
       </c>
       <c r="H166">
-        <v>1</v>
+        <v>1.077756685</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.25">
@@ -5621,10 +5621,10 @@
         <v>296</v>
       </c>
       <c r="G167">
-        <v>5</v>
+        <v>4.7197319719999999</v>
       </c>
       <c r="H167">
-        <v>1</v>
+        <v>0.77023403800000001</v>
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.25">
@@ -5647,10 +5647,10 @@
         <v>294</v>
       </c>
       <c r="G168">
-        <v>2</v>
+        <v>1.9880330289999999</v>
       </c>
       <c r="H168">
-        <v>1</v>
+        <v>1.2674298340000001</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.25">
@@ -5673,10 +5673,10 @@
         <v>294</v>
       </c>
       <c r="G169">
-        <v>3</v>
+        <v>3.1334452229999998</v>
       </c>
       <c r="H169">
-        <v>4</v>
+        <v>4.0401042240000002</v>
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.25">
@@ -5699,10 +5699,10 @@
         <v>295</v>
       </c>
       <c r="G170">
-        <v>2</v>
+        <v>2.2690049719999998</v>
       </c>
       <c r="H170">
-        <v>2</v>
+        <v>1.8186803570000001</v>
       </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.25">
@@ -5725,10 +5725,10 @@
         <v>294</v>
       </c>
       <c r="G171">
-        <v>3</v>
+        <v>3.2973402049999998</v>
       </c>
       <c r="H171">
-        <v>4</v>
+        <v>3.9973628429999999</v>
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.25">
@@ -5751,10 +5751,10 @@
         <v>294</v>
       </c>
       <c r="G172">
-        <v>2</v>
+        <v>2.1094700620000002</v>
       </c>
       <c r="H172">
-        <v>3</v>
+        <v>3.28817563</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.25">
@@ -5777,10 +5777,10 @@
         <v>296</v>
       </c>
       <c r="G173">
-        <v>2</v>
+        <v>2.2850746000000002</v>
       </c>
       <c r="H173">
-        <v>1</v>
+        <v>0.76896681700000002</v>
       </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.25">
@@ -5803,10 +5803,10 @@
         <v>296</v>
       </c>
       <c r="G174">
-        <v>3</v>
+        <v>3.2744787340000001</v>
       </c>
       <c r="H174">
-        <v>1</v>
+        <v>1.269644277</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.25">
@@ -5829,10 +5829,10 @@
         <v>295</v>
       </c>
       <c r="G175">
-        <v>4</v>
+        <v>3.8971351190000001</v>
       </c>
       <c r="H175">
-        <v>4</v>
+        <v>3.758313588</v>
       </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.25">
@@ -5855,10 +5855,10 @@
         <v>296</v>
       </c>
       <c r="G176">
-        <v>4</v>
+        <v>4.2899408140000004</v>
       </c>
       <c r="H176">
-        <v>3</v>
+        <v>3.2918545429999999</v>
       </c>
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.25">
@@ -5881,10 +5881,10 @@
         <v>296</v>
       </c>
       <c r="G177">
-        <v>2</v>
+        <v>2.0866711269999998</v>
       </c>
       <c r="H177">
-        <v>1</v>
+        <v>1.214251448</v>
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.25">
@@ -5907,10 +5907,10 @@
         <v>296</v>
       </c>
       <c r="G178">
-        <v>1</v>
+        <v>1.0324914359999999</v>
       </c>
       <c r="H178">
-        <v>1</v>
+        <v>0.85701606900000005</v>
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.25">
@@ -5933,10 +5933,10 @@
         <v>295</v>
       </c>
       <c r="G179">
-        <v>4</v>
+        <v>4.2939015630000004</v>
       </c>
       <c r="H179">
-        <v>1</v>
+        <v>0.71647882500000004</v>
       </c>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.25">
@@ -5959,10 +5959,10 @@
         <v>295</v>
       </c>
       <c r="G180">
-        <v>4</v>
+        <v>4.0392000259999996</v>
       </c>
       <c r="H180">
-        <v>1</v>
+        <v>0.81290410700000004</v>
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.25">
@@ -5985,10 +5985,10 @@
         <v>294</v>
       </c>
       <c r="G181">
-        <v>5</v>
+        <v>4.898167903</v>
       </c>
       <c r="H181">
-        <v>2</v>
+        <v>1.863337512</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.25">
@@ -6011,10 +6011,10 @@
         <v>296</v>
       </c>
       <c r="G182">
-        <v>5</v>
+        <v>4.9746880950000003</v>
       </c>
       <c r="H182">
-        <v>3</v>
+        <v>2.7648882000000001</v>
       </c>
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.25">
@@ -6037,10 +6037,10 @@
         <v>296</v>
       </c>
       <c r="G183">
-        <v>4</v>
+        <v>3.7043844460000002</v>
       </c>
       <c r="H183">
-        <v>4</v>
+        <v>3.9240879739999999</v>
       </c>
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.25">
@@ -6063,10 +6063,10 @@
         <v>294</v>
       </c>
       <c r="G184">
-        <v>2</v>
+        <v>2.2232534419999999</v>
       </c>
       <c r="H184">
-        <v>4</v>
+        <v>3.8213306089999999</v>
       </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.25">
@@ -6089,10 +6089,10 @@
         <v>296</v>
       </c>
       <c r="G185">
-        <v>5</v>
+        <v>4.735477425</v>
       </c>
       <c r="H185">
-        <v>3</v>
+        <v>2.778595503</v>
       </c>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.25">
@@ -6115,10 +6115,10 @@
         <v>296</v>
       </c>
       <c r="G186">
-        <v>5</v>
+        <v>4.944861285</v>
       </c>
       <c r="H186">
-        <v>1</v>
+        <v>1.1249659839999999</v>
       </c>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.25">
@@ -6141,10 +6141,10 @@
         <v>296</v>
       </c>
       <c r="G187">
-        <v>3</v>
+        <v>3.1848679280000001</v>
       </c>
       <c r="H187">
-        <v>3</v>
+        <v>2.8029120380000001</v>
       </c>
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.25">
@@ -6167,10 +6167,10 @@
         <v>295</v>
       </c>
       <c r="G188">
-        <v>4</v>
+        <v>4.1499197749999999</v>
       </c>
       <c r="H188">
-        <v>4</v>
+        <v>4.2210446709999996</v>
       </c>
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.25">
@@ -6193,10 +6193,10 @@
         <v>295</v>
       </c>
       <c r="G189">
-        <v>5</v>
+        <v>4.7816333850000001</v>
       </c>
       <c r="H189">
-        <v>5</v>
+        <v>4.755329186</v>
       </c>
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.25">
@@ -6219,10 +6219,10 @@
         <v>296</v>
       </c>
       <c r="G190">
-        <v>3</v>
+        <v>3.1185207020000001</v>
       </c>
       <c r="H190">
-        <v>2</v>
+        <v>1.748151413</v>
       </c>
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.25">
@@ -6245,10 +6245,10 @@
         <v>296</v>
       </c>
       <c r="G191">
-        <v>5</v>
+        <v>4.992111972</v>
       </c>
       <c r="H191">
-        <v>4</v>
+        <v>3.8418535459999998</v>
       </c>
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.25">
@@ -6271,10 +6271,10 @@
         <v>296</v>
       </c>
       <c r="G192">
-        <v>3</v>
+        <v>2.7244818080000002</v>
       </c>
       <c r="H192">
-        <v>3</v>
+        <v>2.8607323130000002</v>
       </c>
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.25">
@@ -6297,10 +6297,10 @@
         <v>294</v>
       </c>
       <c r="G193">
-        <v>2</v>
+        <v>1.889695404</v>
       </c>
       <c r="H193">
-        <v>4</v>
+        <v>3.9429707820000002</v>
       </c>
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.25">
@@ -6323,10 +6323,10 @@
         <v>296</v>
       </c>
       <c r="G194">
-        <v>4</v>
+        <v>3.7062740199999999</v>
       </c>
       <c r="H194">
-        <v>2</v>
+        <v>2.1793809500000001</v>
       </c>
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.25">
@@ -6349,10 +6349,10 @@
         <v>296</v>
       </c>
       <c r="G195">
-        <v>4</v>
+        <v>4.1532215859999999</v>
       </c>
       <c r="H195">
-        <v>3</v>
+        <v>3.1178563050000001</v>
       </c>
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.25">
@@ -6375,10 +6375,10 @@
         <v>296</v>
       </c>
       <c r="G196">
-        <v>4</v>
+        <v>3.8431273890000002</v>
       </c>
       <c r="H196">
-        <v>3</v>
+        <v>3.2319060080000002</v>
       </c>
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.25">
@@ -6401,10 +6401,10 @@
         <v>296</v>
       </c>
       <c r="G197">
-        <v>4</v>
+        <v>4.257796602</v>
       </c>
       <c r="H197">
-        <v>2</v>
+        <v>2.1629181169999998</v>
       </c>
     </row>
     <row r="198" spans="1:8" x14ac:dyDescent="0.25">
@@ -6427,10 +6427,10 @@
         <v>296</v>
       </c>
       <c r="G198">
-        <v>2</v>
+        <v>1.8385489290000001</v>
       </c>
       <c r="H198">
-        <v>1</v>
+        <v>1.093361236</v>
       </c>
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.25">
@@ -6453,10 +6453,10 @@
         <v>296</v>
       </c>
       <c r="G199">
-        <v>5</v>
+        <v>4.8725973829999996</v>
       </c>
       <c r="H199">
-        <v>3</v>
+        <v>3.034999821</v>
       </c>
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.25">
@@ -6479,10 +6479,10 @@
         <v>296</v>
       </c>
       <c r="G200">
-        <v>5</v>
+        <v>4.8663837750000001</v>
       </c>
       <c r="H200">
-        <v>5</v>
+        <v>4.8199873650000002</v>
       </c>
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.25">
@@ -6505,10 +6505,10 @@
         <v>296</v>
       </c>
       <c r="G201">
-        <v>3</v>
+        <v>2.9782484359999999</v>
       </c>
       <c r="H201">
-        <v>2</v>
+        <v>2.1848329620000002</v>
       </c>
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.25">
@@ -6531,10 +6531,10 @@
         <v>296</v>
       </c>
       <c r="G202">
-        <v>3</v>
+        <v>3.2150063910000002</v>
       </c>
       <c r="H202">
-        <v>2</v>
+        <v>2.2025412800000002</v>
       </c>
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.25">
@@ -6557,10 +6557,10 @@
         <v>296</v>
       </c>
       <c r="G203">
-        <v>3</v>
+        <v>2.964895657</v>
       </c>
       <c r="H203">
-        <v>4</v>
+        <v>4.1750371480000004</v>
       </c>
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.25">
@@ -6583,10 +6583,10 @@
         <v>296</v>
       </c>
       <c r="G204">
-        <v>5</v>
+        <v>4.9591790099999997</v>
       </c>
       <c r="H204">
-        <v>4</v>
+        <v>3.7342435420000002</v>
       </c>
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.25">
@@ -6609,10 +6609,10 @@
         <v>296</v>
       </c>
       <c r="G205">
-        <v>2</v>
+        <v>2.0725990510000001</v>
       </c>
       <c r="H205">
-        <v>3</v>
+        <v>2.8158268579999999</v>
       </c>
     </row>
     <row r="206" spans="1:8" x14ac:dyDescent="0.25">
@@ -6635,10 +6635,10 @@
         <v>296</v>
       </c>
       <c r="G206">
-        <v>5</v>
+        <v>4.8602629740000003</v>
       </c>
       <c r="H206">
-        <v>1</v>
+        <v>0.97228984200000002</v>
       </c>
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.25">
@@ -6661,10 +6661,10 @@
         <v>296</v>
       </c>
       <c r="G207">
-        <v>5</v>
+        <v>4.9630797419999997</v>
       </c>
       <c r="H207">
-        <v>2</v>
+        <v>2.1195874849999998</v>
       </c>
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.25">
@@ -6687,10 +6687,10 @@
         <v>296</v>
       </c>
       <c r="G208">
-        <v>3</v>
+        <v>2.8310521070000001</v>
       </c>
       <c r="H208">
-        <v>4</v>
+        <v>4.0595095859999999</v>
       </c>
     </row>
     <row r="209" spans="1:8" x14ac:dyDescent="0.25">
@@ -6713,10 +6713,10 @@
         <v>296</v>
       </c>
       <c r="G209">
-        <v>2</v>
+        <v>1.922707197</v>
       </c>
       <c r="H209">
-        <v>4</v>
+        <v>3.8330248579999999</v>
       </c>
     </row>
     <row r="210" spans="1:8" x14ac:dyDescent="0.25">
@@ -6739,10 +6739,10 @@
         <v>296</v>
       </c>
       <c r="G210">
-        <v>5</v>
+        <v>4.9333380160000004</v>
       </c>
       <c r="H210">
-        <v>1</v>
+        <v>0.84803326199999995</v>
       </c>
     </row>
     <row r="211" spans="1:8" x14ac:dyDescent="0.25">
@@ -6765,10 +6765,10 @@
         <v>296</v>
       </c>
       <c r="G211">
-        <v>5</v>
+        <v>4.9089534889999999</v>
       </c>
       <c r="H211">
-        <v>1</v>
+        <v>1.126746287</v>
       </c>
     </row>
     <row r="212" spans="1:8" x14ac:dyDescent="0.25">
@@ -6791,10 +6791,10 @@
         <v>296</v>
       </c>
       <c r="G212">
-        <v>3</v>
+        <v>3.002738028</v>
       </c>
       <c r="H212">
-        <v>1</v>
+        <v>0.93862873099999999</v>
       </c>
     </row>
     <row r="213" spans="1:8" x14ac:dyDescent="0.25">
@@ -6817,10 +6817,10 @@
         <v>296</v>
       </c>
       <c r="G213">
-        <v>4</v>
+        <v>3.7666539779999999</v>
       </c>
       <c r="H213">
-        <v>1</v>
+        <v>0.72728760199999998</v>
       </c>
     </row>
     <row r="214" spans="1:8" x14ac:dyDescent="0.25">
@@ -6843,10 +6843,10 @@
         <v>296</v>
       </c>
       <c r="G214">
-        <v>3</v>
+        <v>3.0183246439999998</v>
       </c>
       <c r="H214">
-        <v>3</v>
+        <v>2.7653234179999999</v>
       </c>
     </row>
     <row r="215" spans="1:8" x14ac:dyDescent="0.25">
@@ -6869,7 +6869,7 @@
         <v>296</v>
       </c>
       <c r="G215">
-        <v>3</v>
+        <v>3.177169487</v>
       </c>
       <c r="H215">
         <v>5</v>
@@ -6895,10 +6895,10 @@
         <v>296</v>
       </c>
       <c r="G216">
-        <v>5</v>
+        <v>4.902268361</v>
       </c>
       <c r="H216">
-        <v>4</v>
+        <v>3.75431735</v>
       </c>
     </row>
     <row r="217" spans="1:8" x14ac:dyDescent="0.25">
@@ -6921,10 +6921,10 @@
         <v>296</v>
       </c>
       <c r="G217">
-        <v>3</v>
+        <v>3.1604196</v>
       </c>
       <c r="H217">
-        <v>3</v>
+        <v>2.8366060360000001</v>
       </c>
     </row>
     <row r="218" spans="1:8" x14ac:dyDescent="0.25">
@@ -6947,10 +6947,10 @@
         <v>296</v>
       </c>
       <c r="G218">
-        <v>3</v>
+        <v>2.7559751800000001</v>
       </c>
       <c r="H218">
-        <v>2</v>
+        <v>2.201670579</v>
       </c>
     </row>
     <row r="219" spans="1:8" x14ac:dyDescent="0.25">
@@ -6973,10 +6973,10 @@
         <v>296</v>
       </c>
       <c r="G219">
-        <v>5</v>
+        <v>4.8297340440000003</v>
       </c>
       <c r="H219">
-        <v>1</v>
+        <v>1.204721774</v>
       </c>
     </row>
     <row r="220" spans="1:8" x14ac:dyDescent="0.25">
@@ -6999,10 +6999,10 @@
         <v>296</v>
       </c>
       <c r="G220">
-        <v>3</v>
+        <v>2.9298393410000001</v>
       </c>
       <c r="H220">
-        <v>4</v>
+        <v>3.8408387880000001</v>
       </c>
     </row>
     <row r="221" spans="1:8" x14ac:dyDescent="0.25">
@@ -7025,10 +7025,10 @@
         <v>296</v>
       </c>
       <c r="G221">
-        <v>5</v>
+        <v>4.8913127349999996</v>
       </c>
       <c r="H221">
-        <v>5</v>
+        <v>4.9961616319999997</v>
       </c>
     </row>
     <row r="222" spans="1:8" x14ac:dyDescent="0.25">
@@ -7051,10 +7051,10 @@
         <v>296</v>
       </c>
       <c r="G222">
-        <v>4</v>
+        <v>4.2317477950000004</v>
       </c>
       <c r="H222">
-        <v>5</v>
+        <v>4.7306837359999996</v>
       </c>
     </row>
     <row r="223" spans="1:8" x14ac:dyDescent="0.25">
@@ -7077,10 +7077,10 @@
         <v>296</v>
       </c>
       <c r="G223">
-        <v>5</v>
+        <v>4.959090379</v>
       </c>
       <c r="H223">
-        <v>4</v>
+        <v>3.7648840739999998</v>
       </c>
     </row>
     <row r="224" spans="1:8" x14ac:dyDescent="0.25">
@@ -7103,10 +7103,10 @@
         <v>296</v>
       </c>
       <c r="G224">
-        <v>5</v>
+        <v>4.7375467819999999</v>
       </c>
       <c r="H224">
-        <v>4</v>
+        <v>4.2153358460000003</v>
       </c>
     </row>
     <row r="225" spans="1:8" x14ac:dyDescent="0.25">
@@ -7129,10 +7129,10 @@
         <v>296</v>
       </c>
       <c r="G225">
-        <v>4</v>
+        <v>4.029429382</v>
       </c>
       <c r="H225">
-        <v>4</v>
+        <v>4.165431559</v>
       </c>
     </row>
     <row r="226" spans="1:8" x14ac:dyDescent="0.25">
@@ -7155,7 +7155,7 @@
         <v>296</v>
       </c>
       <c r="G226">
-        <v>5</v>
+        <v>4.7320407060000003</v>
       </c>
       <c r="H226">
         <v>5</v>
@@ -7181,10 +7181,10 @@
         <v>296</v>
       </c>
       <c r="G227">
-        <v>4</v>
+        <v>4.2334541080000001</v>
       </c>
       <c r="H227">
-        <v>3</v>
+        <v>3.0019016870000002</v>
       </c>
     </row>
     <row r="228" spans="1:8" x14ac:dyDescent="0.25">
@@ -7207,10 +7207,10 @@
         <v>296</v>
       </c>
       <c r="G228">
-        <v>4</v>
+        <v>3.9664689200000001</v>
       </c>
       <c r="H228">
-        <v>1</v>
+        <v>1.256298591</v>
       </c>
     </row>
     <row r="229" spans="1:8" x14ac:dyDescent="0.25">
@@ -7233,10 +7233,10 @@
         <v>296</v>
       </c>
       <c r="G229">
-        <v>5</v>
+        <v>4.7327647979999998</v>
       </c>
       <c r="H229">
-        <v>5</v>
+        <v>4.8271081120000003</v>
       </c>
     </row>
     <row r="230" spans="1:8" x14ac:dyDescent="0.25">
@@ -7259,10 +7259,10 @@
         <v>295</v>
       </c>
       <c r="G230">
-        <v>2</v>
+        <v>1.9413113639999999</v>
       </c>
       <c r="H230">
-        <v>4</v>
+        <v>4.2423185309999996</v>
       </c>
     </row>
     <row r="231" spans="1:8" x14ac:dyDescent="0.25">
@@ -7285,10 +7285,10 @@
         <v>296</v>
       </c>
       <c r="G231">
-        <v>3</v>
+        <v>2.976366617</v>
       </c>
       <c r="H231">
-        <v>1</v>
+        <v>1.2607080820000001</v>
       </c>
     </row>
     <row r="232" spans="1:8" x14ac:dyDescent="0.25">
@@ -7311,10 +7311,10 @@
         <v>296</v>
       </c>
       <c r="G232">
-        <v>5</v>
+        <v>4.8526676850000001</v>
       </c>
       <c r="H232">
-        <v>1</v>
+        <v>0.78987312600000004</v>
       </c>
     </row>
     <row r="233" spans="1:8" x14ac:dyDescent="0.25">
@@ -7337,10 +7337,10 @@
         <v>295</v>
       </c>
       <c r="G233">
-        <v>2</v>
+        <v>1.752277426</v>
       </c>
       <c r="H233">
-        <v>2</v>
+        <v>1.723953045</v>
       </c>
     </row>
     <row r="234" spans="1:8" x14ac:dyDescent="0.25">
@@ -7363,10 +7363,10 @@
         <v>296</v>
       </c>
       <c r="G234">
-        <v>4</v>
+        <v>3.7947864029999998</v>
       </c>
       <c r="H234">
-        <v>5</v>
+        <v>4.919244892</v>
       </c>
     </row>
     <row r="235" spans="1:8" x14ac:dyDescent="0.25">
@@ -7389,10 +7389,10 @@
         <v>296</v>
       </c>
       <c r="G235">
-        <v>3</v>
+        <v>3.0185239749999999</v>
       </c>
       <c r="H235">
-        <v>1</v>
+        <v>1.1039449180000001</v>
       </c>
     </row>
     <row r="236" spans="1:8" x14ac:dyDescent="0.25">
@@ -7415,10 +7415,10 @@
         <v>295</v>
       </c>
       <c r="G236">
-        <v>3</v>
+        <v>2.8649255060000001</v>
       </c>
       <c r="H236">
-        <v>2</v>
+        <v>1.957162163</v>
       </c>
     </row>
     <row r="237" spans="1:8" x14ac:dyDescent="0.25">
@@ -7441,10 +7441,10 @@
         <v>296</v>
       </c>
       <c r="G237">
-        <v>3</v>
+        <v>3.235382398</v>
       </c>
       <c r="H237">
-        <v>2</v>
+        <v>1.902168496</v>
       </c>
     </row>
     <row r="238" spans="1:8" x14ac:dyDescent="0.25">
@@ -7467,10 +7467,10 @@
         <v>296</v>
       </c>
       <c r="G238">
-        <v>3</v>
+        <v>2.9747024930000001</v>
       </c>
       <c r="H238">
-        <v>2</v>
+        <v>1.972529051</v>
       </c>
     </row>
     <row r="239" spans="1:8" x14ac:dyDescent="0.25">
@@ -7493,10 +7493,10 @@
         <v>296</v>
       </c>
       <c r="G239">
-        <v>3</v>
+        <v>2.882231032</v>
       </c>
       <c r="H239">
-        <v>3</v>
+        <v>2.9105793169999998</v>
       </c>
     </row>
     <row r="240" spans="1:8" x14ac:dyDescent="0.25">
@@ -7519,10 +7519,10 @@
         <v>296</v>
       </c>
       <c r="G240">
-        <v>5</v>
+        <v>4.9828393499999999</v>
       </c>
       <c r="H240">
-        <v>4</v>
+        <v>4.1578441960000001</v>
       </c>
     </row>
     <row r="241" spans="1:8" x14ac:dyDescent="0.25">
@@ -7545,10 +7545,10 @@
         <v>296</v>
       </c>
       <c r="G241">
-        <v>4</v>
+        <v>3.8005865129999998</v>
       </c>
       <c r="H241">
-        <v>2</v>
+        <v>2.1651465070000002</v>
       </c>
     </row>
     <row r="242" spans="1:8" x14ac:dyDescent="0.25">
@@ -7571,10 +7571,10 @@
         <v>296</v>
       </c>
       <c r="G242">
-        <v>4</v>
+        <v>4.1967770639999999</v>
       </c>
       <c r="H242">
-        <v>4</v>
+        <v>3.7625736160000001</v>
       </c>
     </row>
     <row r="243" spans="1:8" x14ac:dyDescent="0.25">
@@ -7597,10 +7597,10 @@
         <v>296</v>
       </c>
       <c r="G243">
-        <v>4</v>
+        <v>4.2598969340000004</v>
       </c>
       <c r="H243">
-        <v>2</v>
+        <v>2.1170005270000001</v>
       </c>
     </row>
     <row r="244" spans="1:8" x14ac:dyDescent="0.25">
@@ -7623,10 +7623,10 @@
         <v>296</v>
       </c>
       <c r="G244">
-        <v>4</v>
+        <v>3.807302892</v>
       </c>
       <c r="H244">
-        <v>2</v>
+        <v>2.0805438679999999</v>
       </c>
     </row>
     <row r="245" spans="1:8" x14ac:dyDescent="0.25">
@@ -7649,10 +7649,10 @@
         <v>296</v>
       </c>
       <c r="G245">
-        <v>3</v>
+        <v>3.14710533</v>
       </c>
       <c r="H245">
-        <v>3</v>
+        <v>2.8839111650000002</v>
       </c>
     </row>
     <row r="246" spans="1:8" x14ac:dyDescent="0.25">
@@ -7675,10 +7675,10 @@
         <v>296</v>
       </c>
       <c r="G246">
-        <v>4</v>
+        <v>4.1462134720000003</v>
       </c>
       <c r="H246">
-        <v>1</v>
+        <v>1.248368549</v>
       </c>
     </row>
     <row r="247" spans="1:8" x14ac:dyDescent="0.25">
@@ -7701,10 +7701,10 @@
         <v>296</v>
       </c>
       <c r="G247">
-        <v>5</v>
+        <v>4.9468592060000001</v>
       </c>
       <c r="H247">
-        <v>3</v>
+        <v>2.957994776</v>
       </c>
     </row>
     <row r="248" spans="1:8" x14ac:dyDescent="0.25">
@@ -7727,10 +7727,10 @@
         <v>296</v>
       </c>
       <c r="G248">
-        <v>3</v>
+        <v>2.871451483</v>
       </c>
       <c r="H248">
-        <v>2</v>
+        <v>1.8054380990000001</v>
       </c>
     </row>
     <row r="249" spans="1:8" x14ac:dyDescent="0.25">
@@ -7753,10 +7753,10 @@
         <v>296</v>
       </c>
       <c r="G249">
-        <v>3</v>
+        <v>3.149467198</v>
       </c>
       <c r="H249">
-        <v>1</v>
+        <v>0.90740004699999999</v>
       </c>
     </row>
     <row r="250" spans="1:8" x14ac:dyDescent="0.25">
@@ -7779,10 +7779,10 @@
         <v>296</v>
       </c>
       <c r="G250">
-        <v>3</v>
+        <v>3.0857625319999999</v>
       </c>
       <c r="H250">
-        <v>1</v>
+        <v>0.91024130800000003</v>
       </c>
     </row>
     <row r="251" spans="1:8" x14ac:dyDescent="0.25">
@@ -7805,10 +7805,10 @@
         <v>296</v>
       </c>
       <c r="G251">
-        <v>3</v>
+        <v>3.0816771410000001</v>
       </c>
       <c r="H251">
-        <v>2</v>
+        <v>2.0999355460000002</v>
       </c>
     </row>
     <row r="252" spans="1:8" x14ac:dyDescent="0.25">
@@ -7831,10 +7831,10 @@
         <v>295</v>
       </c>
       <c r="G252">
-        <v>2</v>
+        <v>2.0495783360000002</v>
       </c>
       <c r="H252">
-        <v>1</v>
+        <v>1.1108774610000001</v>
       </c>
     </row>
     <row r="253" spans="1:8" x14ac:dyDescent="0.25">
@@ -7857,10 +7857,10 @@
         <v>295</v>
       </c>
       <c r="G253">
-        <v>3</v>
+        <v>3.1573397120000002</v>
       </c>
       <c r="H253">
-        <v>3</v>
+        <v>2.8984864369999999</v>
       </c>
     </row>
     <row r="254" spans="1:8" x14ac:dyDescent="0.25">
@@ -7883,10 +7883,10 @@
         <v>296</v>
       </c>
       <c r="G254">
-        <v>3</v>
+        <v>2.8265563579999999</v>
       </c>
       <c r="H254">
-        <v>3</v>
+        <v>2.8608962870000001</v>
       </c>
     </row>
     <row r="255" spans="1:8" x14ac:dyDescent="0.25">
@@ -7909,10 +7909,10 @@
         <v>296</v>
       </c>
       <c r="G255">
-        <v>4</v>
+        <v>4.0043299179999998</v>
       </c>
       <c r="H255">
-        <v>1</v>
+        <v>1.2059609039999999</v>
       </c>
     </row>
     <row r="256" spans="1:8" x14ac:dyDescent="0.25">
@@ -7935,10 +7935,10 @@
         <v>296</v>
       </c>
       <c r="G256">
-        <v>3</v>
+        <v>3.2027383249999999</v>
       </c>
       <c r="H256">
-        <v>1</v>
+        <v>0.74796043700000003</v>
       </c>
     </row>
     <row r="257" spans="1:8" x14ac:dyDescent="0.25">
@@ -7961,10 +7961,10 @@
         <v>296</v>
       </c>
       <c r="G257">
-        <v>5</v>
+        <v>4.9787507719999997</v>
       </c>
       <c r="H257">
-        <v>4</v>
+        <v>4.0472283840000003</v>
       </c>
     </row>
     <row r="258" spans="1:8" x14ac:dyDescent="0.25">
@@ -7987,10 +7987,10 @@
         <v>296</v>
       </c>
       <c r="G258">
-        <v>4</v>
+        <v>4.0092266849999998</v>
       </c>
       <c r="H258">
-        <v>3</v>
+        <v>2.8328176439999999</v>
       </c>
     </row>
     <row r="259" spans="1:8" x14ac:dyDescent="0.25">
@@ -8013,10 +8013,10 @@
         <v>296</v>
       </c>
       <c r="G259">
-        <v>4</v>
+        <v>4.1759317469999999</v>
       </c>
       <c r="H259">
-        <v>5</v>
+        <v>4.9169502610000002</v>
       </c>
     </row>
     <row r="260" spans="1:8" x14ac:dyDescent="0.25">
@@ -8039,10 +8039,10 @@
         <v>296</v>
       </c>
       <c r="G260">
-        <v>4</v>
+        <v>4.22603507</v>
       </c>
       <c r="H260">
-        <v>4</v>
+        <v>3.9161223079999998</v>
       </c>
     </row>
     <row r="261" spans="1:8" x14ac:dyDescent="0.25">
@@ -8065,10 +8065,10 @@
         <v>296</v>
       </c>
       <c r="G261">
-        <v>5</v>
+        <v>4.8258685669999997</v>
       </c>
       <c r="H261">
-        <v>4</v>
+        <v>4.0533718509999996</v>
       </c>
     </row>
     <row r="262" spans="1:8" x14ac:dyDescent="0.25">
@@ -8091,10 +8091,10 @@
         <v>296</v>
       </c>
       <c r="G262">
-        <v>5</v>
+        <v>4.8525494629999999</v>
       </c>
       <c r="H262">
-        <v>3</v>
+        <v>3.2442657110000002</v>
       </c>
     </row>
     <row r="263" spans="1:8" x14ac:dyDescent="0.25">
@@ -8117,10 +8117,10 @@
         <v>295</v>
       </c>
       <c r="G263">
-        <v>5</v>
+        <v>4.8149306259999998</v>
       </c>
       <c r="H263">
-        <v>5</v>
+        <v>4.7774843579999997</v>
       </c>
     </row>
     <row r="264" spans="1:8" x14ac:dyDescent="0.25">
@@ -8143,10 +8143,10 @@
         <v>296</v>
       </c>
       <c r="G264">
-        <v>5</v>
+        <v>4.7348140839999999</v>
       </c>
       <c r="H264">
-        <v>2</v>
+        <v>1.8751526489999999</v>
       </c>
     </row>
     <row r="265" spans="1:8" x14ac:dyDescent="0.25">
@@ -8169,10 +8169,10 @@
         <v>295</v>
       </c>
       <c r="G265">
-        <v>5</v>
+        <v>4.7365481689999998</v>
       </c>
       <c r="H265">
-        <v>5</v>
+        <v>4.8484450360000002</v>
       </c>
     </row>
     <row r="266" spans="1:8" x14ac:dyDescent="0.25">
@@ -8195,7 +8195,7 @@
         <v>294</v>
       </c>
       <c r="G266">
-        <v>5</v>
+        <v>4.7455189840000003</v>
       </c>
       <c r="H266">
         <v>5</v>
@@ -8221,10 +8221,10 @@
         <v>294</v>
       </c>
       <c r="G267">
-        <v>5</v>
+        <v>4.9154860710000001</v>
       </c>
       <c r="H267">
-        <v>5</v>
+        <v>4.8860533659999996</v>
       </c>
     </row>
     <row r="268" spans="1:8" x14ac:dyDescent="0.25">
@@ -8247,10 +8247,10 @@
         <v>296</v>
       </c>
       <c r="G268">
-        <v>5</v>
+        <v>4.8401987489999998</v>
       </c>
       <c r="H268">
-        <v>5</v>
+        <v>4.7605647930000003</v>
       </c>
     </row>
     <row r="269" spans="1:8" x14ac:dyDescent="0.25">
@@ -8273,10 +8273,10 @@
         <v>296</v>
       </c>
       <c r="G269">
-        <v>5</v>
+        <v>4.712324422</v>
       </c>
       <c r="H269">
-        <v>5</v>
+        <v>4.9495527800000003</v>
       </c>
     </row>
     <row r="270" spans="1:8" x14ac:dyDescent="0.25">
@@ -8299,10 +8299,10 @@
         <v>296</v>
       </c>
       <c r="G270">
-        <v>5</v>
+        <v>4.941744785</v>
       </c>
       <c r="H270">
-        <v>5</v>
+        <v>4.9518088210000002</v>
       </c>
     </row>
     <row r="271" spans="1:8" x14ac:dyDescent="0.25">
@@ -8325,10 +8325,10 @@
         <v>296</v>
       </c>
       <c r="G271">
-        <v>5</v>
+        <v>4.969829099</v>
       </c>
       <c r="H271">
-        <v>5</v>
+        <v>4.7442240059999996</v>
       </c>
     </row>
     <row r="272" spans="1:8" x14ac:dyDescent="0.25">
@@ -8354,7 +8354,7 @@
         <v>5</v>
       </c>
       <c r="H272">
-        <v>5</v>
+        <v>4.7360257959999998</v>
       </c>
     </row>
     <row r="273" spans="1:8" x14ac:dyDescent="0.25">
@@ -8377,10 +8377,10 @@
         <v>296</v>
       </c>
       <c r="G273">
-        <v>5</v>
+        <v>4.9043403909999999</v>
       </c>
       <c r="H273">
-        <v>3</v>
+        <v>2.9105158250000001</v>
       </c>
     </row>
     <row r="274" spans="1:8" x14ac:dyDescent="0.25">
@@ -8403,10 +8403,10 @@
         <v>295</v>
       </c>
       <c r="G274">
-        <v>5</v>
+        <v>4.996860055</v>
       </c>
       <c r="H274">
-        <v>4</v>
+        <v>3.7323541260000002</v>
       </c>
     </row>
     <row r="275" spans="1:8" x14ac:dyDescent="0.25">
@@ -8429,10 +8429,10 @@
         <v>295</v>
       </c>
       <c r="G275">
-        <v>5</v>
+        <v>4.8099641139999996</v>
       </c>
       <c r="H275">
-        <v>4</v>
+        <v>4.1820075550000002</v>
       </c>
     </row>
     <row r="276" spans="1:8" x14ac:dyDescent="0.25">
@@ -8455,10 +8455,10 @@
         <v>295</v>
       </c>
       <c r="G276">
-        <v>5</v>
+        <v>4.7658854079999999</v>
       </c>
       <c r="H276">
-        <v>4</v>
+        <v>4.1359092889999998</v>
       </c>
     </row>
     <row r="277" spans="1:8" x14ac:dyDescent="0.25">
@@ -8481,10 +8481,10 @@
         <v>295</v>
       </c>
       <c r="G277">
-        <v>5</v>
+        <v>4.8953856699999996</v>
       </c>
       <c r="H277">
-        <v>4</v>
+        <v>4.1824096910000002</v>
       </c>
     </row>
     <row r="278" spans="1:8" x14ac:dyDescent="0.25">
@@ -8507,10 +8507,10 @@
         <v>294</v>
       </c>
       <c r="G278">
-        <v>4</v>
+        <v>3.7597869689999999</v>
       </c>
       <c r="H278">
-        <v>4</v>
+        <v>3.7517351250000002</v>
       </c>
     </row>
     <row r="279" spans="1:8" x14ac:dyDescent="0.25">
@@ -8533,10 +8533,10 @@
         <v>294</v>
       </c>
       <c r="G279">
-        <v>5</v>
+        <v>4.8913451190000004</v>
       </c>
       <c r="H279">
-        <v>5</v>
+        <v>4.8967406020000004</v>
       </c>
     </row>
     <row r="280" spans="1:8" x14ac:dyDescent="0.25">
@@ -8559,10 +8559,10 @@
         <v>295</v>
       </c>
       <c r="G280">
-        <v>3</v>
+        <v>2.8274448520000002</v>
       </c>
       <c r="H280">
-        <v>5</v>
+        <v>4.9801319680000002</v>
       </c>
     </row>
     <row r="281" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>